<commit_message>
Actualizacion Historia de Usuario
</commit_message>
<xml_diff>
--- a/DOCUMENTACION/ELICITACION/1.3 HISTORIAS DE USUARIO/G8_HISTORIA DE USUARIO_V6.0.xlsx
+++ b/DOCUMENTACION/ELICITACION/1.3 HISTORIAS DE USUARIO/G8_HISTORIA DE USUARIO_V6.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G403\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81B0ED55-0821-4A54-BF51-04DA1D7915CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2F6AAE-2CA9-48C7-B195-EB89AECC28EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -807,56 +807,6 @@
     <xf numFmtId="164" fontId="17" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -866,6 +816,56 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1208,8 +1208,8 @@
   </sheetPr>
   <dimension ref="A1:O992"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1237,22 +1237,22 @@
       <c r="L2" s="3"/>
     </row>
     <row r="3" spans="1:15" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H4" s="4"/>
@@ -1311,43 +1311,43 @@
       <c r="B6" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="62" t="s">
+      <c r="C6" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="D6" s="64" t="s">
+      <c r="D6" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="64" t="s">
+      <c r="E6" s="36" t="s">
         <v>72</v>
       </c>
       <c r="F6" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="G6" s="64" t="s">
+      <c r="G6" s="36" t="s">
         <v>73</v>
       </c>
       <c r="H6" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="I6" s="62" t="s">
+      <c r="I6" s="34" t="s">
         <v>42</v>
       </c>
       <c r="J6" s="33">
-        <v>45488</v>
-      </c>
-      <c r="K6" s="63" t="s">
+        <v>45481</v>
+      </c>
+      <c r="K6" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="L6" s="63" t="s">
+      <c r="L6" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="64" t="s">
+      <c r="M6" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="N6" s="64" t="s">
+      <c r="N6" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="O6" s="64" t="s">
+      <c r="O6" s="36" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1612,366 +1612,366 @@
       <c r="L21" s="3"/>
     </row>
     <row r="22" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="36"/>
-      <c r="C22" s="36"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="39"/>
+      <c r="E22" s="39"/>
+      <c r="F22" s="39"/>
+      <c r="G22" s="39"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="39"/>
+      <c r="J22" s="39"/>
       <c r="K22" s="2"/>
       <c r="L22" s="3"/>
     </row>
     <row r="23" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="36"/>
-      <c r="C23" s="36"/>
-      <c r="D23" s="36"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
       <c r="K23" s="2"/>
       <c r="L23" s="3"/>
     </row>
     <row r="24" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="36"/>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
       <c r="K24" s="2"/>
       <c r="L24" s="3"/>
     </row>
     <row r="25" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="36"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="36"/>
-      <c r="I25" s="36"/>
-      <c r="J25" s="36"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="39"/>
+      <c r="H25" s="39"/>
+      <c r="I25" s="39"/>
+      <c r="J25" s="39"/>
       <c r="K25" s="2"/>
       <c r="L25" s="3"/>
     </row>
     <row r="26" spans="2:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="36"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
+      <c r="B26" s="39"/>
+      <c r="C26" s="39"/>
+      <c r="D26" s="39"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="39"/>
+      <c r="H26" s="39"/>
+      <c r="I26" s="39"/>
+      <c r="J26" s="39"/>
       <c r="K26" s="2"/>
       <c r="L26" s="3"/>
     </row>
     <row r="27" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="39"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
+      <c r="J27" s="39"/>
       <c r="K27" s="2"/>
       <c r="L27" s="3"/>
     </row>
     <row r="28" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
+      <c r="G28" s="39"/>
+      <c r="H28" s="39"/>
+      <c r="I28" s="39"/>
+      <c r="J28" s="39"/>
       <c r="K28" s="2"/>
       <c r="L28" s="3"/>
     </row>
     <row r="29" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="36"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="36"/>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
       <c r="K29" s="2"/>
       <c r="L29" s="3"/>
     </row>
     <row r="30" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="36"/>
-      <c r="C30" s="36"/>
-      <c r="D30" s="36"/>
-      <c r="E30" s="36"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="36"/>
-      <c r="I30" s="36"/>
-      <c r="J30" s="36"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
       <c r="K30" s="2"/>
       <c r="L30" s="3"/>
     </row>
     <row r="31" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="36"/>
-      <c r="C31" s="36"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="36"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="36"/>
-      <c r="I31" s="36"/>
-      <c r="J31" s="36"/>
+      <c r="B31" s="39"/>
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+      <c r="E31" s="39"/>
+      <c r="F31" s="39"/>
+      <c r="G31" s="39"/>
+      <c r="H31" s="39"/>
+      <c r="I31" s="39"/>
+      <c r="J31" s="39"/>
       <c r="K31" s="2"/>
       <c r="L31" s="3"/>
     </row>
     <row r="32" spans="2:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="36"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="36"/>
-      <c r="E32" s="36"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="36"/>
-      <c r="I32" s="36"/>
-      <c r="J32" s="36"/>
+      <c r="B32" s="39"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="39"/>
+      <c r="H32" s="39"/>
+      <c r="I32" s="39"/>
+      <c r="J32" s="39"/>
       <c r="K32" s="2"/>
       <c r="L32" s="3"/>
     </row>
     <row r="33" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="36"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="36"/>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="36"/>
-      <c r="I33" s="36"/>
-      <c r="J33" s="36"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="39"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="39"/>
+      <c r="H33" s="39"/>
+      <c r="I33" s="39"/>
+      <c r="J33" s="39"/>
       <c r="K33" s="2"/>
       <c r="L33" s="3"/>
     </row>
     <row r="34" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="36"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="36"/>
+      <c r="B34" s="39"/>
+      <c r="C34" s="39"/>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="39"/>
+      <c r="J34" s="39"/>
       <c r="K34" s="2"/>
       <c r="L34" s="3"/>
     </row>
     <row r="35" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="36"/>
-      <c r="C35" s="36"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="36"/>
-      <c r="H35" s="36"/>
-      <c r="I35" s="36"/>
-      <c r="J35" s="36"/>
+      <c r="B35" s="39"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+      <c r="I35" s="39"/>
+      <c r="J35" s="39"/>
       <c r="K35" s="2"/>
       <c r="L35" s="3"/>
     </row>
     <row r="36" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="36"/>
+      <c r="B36" s="39"/>
+      <c r="C36" s="39"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="39"/>
+      <c r="H36" s="39"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
       <c r="K36" s="2"/>
       <c r="L36" s="3"/>
     </row>
     <row r="37" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
+      <c r="B37" s="39"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="39"/>
+      <c r="H37" s="39"/>
+      <c r="I37" s="39"/>
+      <c r="J37" s="39"/>
       <c r="K37" s="2"/>
       <c r="L37" s="3"/>
     </row>
     <row r="38" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
+      <c r="B38" s="39"/>
+      <c r="C38" s="39"/>
+      <c r="D38" s="39"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="39"/>
+      <c r="H38" s="39"/>
+      <c r="I38" s="39"/>
+      <c r="J38" s="39"/>
       <c r="K38" s="2"/>
       <c r="L38" s="3"/>
     </row>
     <row r="39" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="36"/>
+      <c r="B39" s="39"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
       <c r="K39" s="2"/>
       <c r="L39" s="3"/>
     </row>
     <row r="40" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
+      <c r="B40" s="39"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="39"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
       <c r="K40" s="2"/>
       <c r="L40" s="3"/>
     </row>
     <row r="41" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="36"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="39"/>
+      <c r="J41" s="39"/>
       <c r="K41" s="2"/>
       <c r="L41" s="3"/>
     </row>
     <row r="42" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="36"/>
+      <c r="B42" s="39"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
       <c r="K42" s="2"/>
       <c r="L42" s="3"/>
     </row>
     <row r="43" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="39"/>
+      <c r="H43" s="39"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
       <c r="K43" s="2"/>
       <c r="L43" s="3"/>
     </row>
     <row r="44" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="39"/>
+      <c r="H44" s="39"/>
+      <c r="I44" s="39"/>
+      <c r="J44" s="39"/>
       <c r="K44" s="2"/>
       <c r="L44" s="3"/>
     </row>
     <row r="45" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="36"/>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="36"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
+      <c r="B45" s="39"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="39"/>
+      <c r="H45" s="39"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
       <c r="K45" s="2"/>
       <c r="L45" s="3"/>
     </row>
     <row r="46" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="36"/>
-      <c r="C46" s="36"/>
-      <c r="D46" s="36"/>
-      <c r="E46" s="36"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="36"/>
-      <c r="H46" s="36"/>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="B46" s="39"/>
+      <c r="C46" s="39"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="39"/>
+      <c r="H46" s="39"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
       <c r="K46" s="2"/>
       <c r="L46" s="3"/>
     </row>
     <row r="47" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="36"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="36"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="39"/>
+      <c r="H47" s="39"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
       <c r="K47" s="2"/>
       <c r="L47" s="3"/>
     </row>
     <row r="48" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="36"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="36"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="36"/>
-      <c r="J48" s="36"/>
+      <c r="B48" s="39"/>
+      <c r="C48" s="39"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="39"/>
+      <c r="I48" s="39"/>
+      <c r="J48" s="39"/>
       <c r="K48" s="2"/>
       <c r="L48" s="3"/>
     </row>
     <row r="49" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="36"/>
-      <c r="C49" s="36"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="36"/>
-      <c r="F49" s="36"/>
-      <c r="G49" s="36"/>
-      <c r="H49" s="36"/>
-      <c r="I49" s="36"/>
-      <c r="J49" s="36"/>
+      <c r="B49" s="39"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="39"/>
+      <c r="I49" s="39"/>
+      <c r="J49" s="39"/>
       <c r="K49" s="2"/>
       <c r="L49" s="3"/>
     </row>
@@ -7661,23 +7661,23 @@
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="2:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="59" t="s">
+      <c r="B6" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="60"/>
-      <c r="N6" s="60"/>
-      <c r="O6" s="60"/>
-      <c r="P6" s="46"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="42"/>
     </row>
     <row r="7" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="8"/>
@@ -7717,15 +7717,15 @@
         <v>0</v>
       </c>
       <c r="D9" s="10"/>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="46"/>
+      <c r="F9" s="42"/>
       <c r="G9" s="10"/>
-      <c r="H9" s="45" t="s">
+      <c r="H9" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="46"/>
+      <c r="I9" s="42"/>
       <c r="J9" s="11"/>
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
@@ -7740,17 +7740,17 @@
         <v>23</v>
       </c>
       <c r="D10" s="13"/>
-      <c r="E10" s="61" t="e">
+      <c r="E10" s="45" t="e">
         <f>VLOOKUP(C10,'Formato descripción HU'!B7:O8,5,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F10" s="46"/>
+      <c r="F10" s="42"/>
       <c r="G10" s="14"/>
-      <c r="H10" s="47" t="e">
+      <c r="H10" s="44" t="e">
         <f>VLOOKUP(C10,'Formato descripción HU'!B7:O8,11,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="I10" s="46"/>
+      <c r="I10" s="42"/>
       <c r="J10" s="14"/>
       <c r="K10" s="11"/>
       <c r="L10" s="11"/>
@@ -7782,15 +7782,15 @@
         <v>24</v>
       </c>
       <c r="D12" s="13"/>
-      <c r="E12" s="45" t="s">
+      <c r="E12" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="46"/>
+      <c r="F12" s="42"/>
       <c r="G12" s="14"/>
-      <c r="H12" s="45" t="s">
+      <c r="H12" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="I12" s="46"/>
+      <c r="I12" s="42"/>
       <c r="J12" s="14"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16"/>
@@ -7806,17 +7806,17 @@
         <v>#N/A</v>
       </c>
       <c r="D13" s="13"/>
-      <c r="E13" s="47" t="e">
+      <c r="E13" s="44" t="e">
         <f>VLOOKUP(C10,'Formato descripción HU'!B7:O8,10,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F13" s="46"/>
+      <c r="F13" s="42"/>
       <c r="G13" s="14"/>
-      <c r="H13" s="47" t="e">
+      <c r="H13" s="44" t="e">
         <f>VLOOKUP(C10,'Formato descripción HU'!B7:O8,7,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="I13" s="46"/>
+      <c r="I13" s="42"/>
       <c r="J13" s="14"/>
       <c r="K13" s="16"/>
       <c r="L13" s="16"/>
@@ -7844,68 +7844,68 @@
     </row>
     <row r="15" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="27"/>
-      <c r="C15" s="48" t="s">
+      <c r="C15" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="37" t="e">
+      <c r="D15" s="56" t="e">
         <f>VLOOKUP(C10,'Formato descripción HU'!B7:O8,3,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="E15" s="39"/>
+      <c r="E15" s="50"/>
       <c r="F15" s="11"/>
-      <c r="G15" s="48" t="s">
+      <c r="G15" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="H15" s="37" t="e">
+      <c r="H15" s="56" t="e">
         <f>VLOOKUP(C10,'Formato descripción HU'!B7:O8,4,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="I15" s="38"/>
-      <c r="J15" s="39"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="50"/>
       <c r="K15" s="11"/>
-      <c r="L15" s="48" t="s">
+      <c r="L15" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="M15" s="37" t="e">
+      <c r="M15" s="56" t="e">
         <f>VLOOKUP(C10,'Formato descripción HU'!B7:O8,6,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="N15" s="38"/>
-      <c r="O15" s="39"/>
+      <c r="N15" s="57"/>
+      <c r="O15" s="50"/>
       <c r="P15" s="28"/>
     </row>
     <row r="16" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="27"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="41"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="55"/>
       <c r="F16" s="11"/>
-      <c r="G16" s="49"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="41"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="55"/>
       <c r="K16" s="11"/>
-      <c r="L16" s="49"/>
-      <c r="M16" s="40"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="41"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="54"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="55"/>
       <c r="P16" s="28"/>
     </row>
     <row r="17" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="27"/>
-      <c r="C17" s="50"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="44"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="52"/>
       <c r="F17" s="11"/>
-      <c r="G17" s="50"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="44"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="52"/>
       <c r="K17" s="11"/>
-      <c r="L17" s="50"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="43"/>
-      <c r="O17" s="44"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="51"/>
+      <c r="N17" s="58"/>
+      <c r="O17" s="52"/>
       <c r="P17" s="28"/>
     </row>
     <row r="18" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7927,41 +7927,41 @@
     </row>
     <row r="19" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="27"/>
-      <c r="C19" s="57" t="s">
+      <c r="C19" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="39"/>
-      <c r="E19" s="51" t="e">
+      <c r="D19" s="50"/>
+      <c r="E19" s="59" t="e">
         <f>VLOOKUP(C10,'Formato descripción HU'!B7:O8,14,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F19" s="52"/>
-      <c r="G19" s="52"/>
-      <c r="H19" s="52"/>
-      <c r="I19" s="52"/>
-      <c r="J19" s="52"/>
-      <c r="K19" s="52"/>
-      <c r="L19" s="52"/>
-      <c r="M19" s="52"/>
-      <c r="N19" s="52"/>
-      <c r="O19" s="53"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="60"/>
+      <c r="M19" s="60"/>
+      <c r="N19" s="60"/>
+      <c r="O19" s="61"/>
       <c r="P19" s="28"/>
     </row>
     <row r="20" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="27"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="54"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="55"/>
-      <c r="J20" s="55"/>
-      <c r="K20" s="55"/>
-      <c r="L20" s="55"/>
-      <c r="M20" s="55"/>
-      <c r="N20" s="55"/>
-      <c r="O20" s="56"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="63"/>
+      <c r="H20" s="63"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="63"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="63"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="64"/>
       <c r="P20" s="28"/>
     </row>
     <row r="21" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -7983,63 +7983,63 @@
     </row>
     <row r="22" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="27"/>
-      <c r="C22" s="58" t="s">
+      <c r="C22" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="37" t="e">
+      <c r="D22" s="50"/>
+      <c r="E22" s="56" t="e">
         <f>VLOOKUP(C10,'Formato descripción HU'!B7:O8,12,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="39"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="50"/>
       <c r="I22" s="11"/>
-      <c r="J22" s="58" t="s">
+      <c r="J22" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="K22" s="39"/>
-      <c r="L22" s="37" t="e">
+      <c r="K22" s="50"/>
+      <c r="L22" s="56" t="e">
         <f>VLOOKUP(C10,'Formato descripción HU'!B7:O8,13,0)</f>
         <v>#N/A</v>
       </c>
-      <c r="M22" s="38"/>
-      <c r="N22" s="38"/>
-      <c r="O22" s="39"/>
+      <c r="M22" s="57"/>
+      <c r="N22" s="57"/>
+      <c r="O22" s="50"/>
       <c r="P22" s="28"/>
     </row>
     <row r="23" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="27"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="41"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="54"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="55"/>
       <c r="I23" s="11"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="40"/>
-      <c r="M23" s="35"/>
-      <c r="N23" s="35"/>
-      <c r="O23" s="41"/>
+      <c r="J23" s="54"/>
+      <c r="K23" s="55"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="55"/>
       <c r="P23" s="28"/>
     </row>
     <row r="24" spans="2:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="27"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="44"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="52"/>
       <c r="I24" s="11"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="44"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="43"/>
-      <c r="N24" s="43"/>
-      <c r="O24" s="44"/>
+      <c r="J24" s="51"/>
+      <c r="K24" s="52"/>
+      <c r="L24" s="51"/>
+      <c r="M24" s="58"/>
+      <c r="N24" s="58"/>
+      <c r="O24" s="52"/>
       <c r="P24" s="28"/>
     </row>
     <row r="25" spans="2:16" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9056,17 +9056,6 @@
     <row r="1020" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B6:P6"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C19:D20"/>
-    <mergeCell ref="C22:D24"/>
-    <mergeCell ref="E22:H24"/>
-    <mergeCell ref="J22:K24"/>
     <mergeCell ref="L22:O24"/>
     <mergeCell ref="H12:I12"/>
     <mergeCell ref="H13:I13"/>
@@ -9077,6 +9066,17 @@
     <mergeCell ref="M15:O17"/>
     <mergeCell ref="E19:O20"/>
     <mergeCell ref="E13:F13"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="C19:D20"/>
+    <mergeCell ref="C22:D24"/>
+    <mergeCell ref="E22:H24"/>
+    <mergeCell ref="J22:K24"/>
+    <mergeCell ref="B6:P6"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E10:F10"/>
   </mergeCells>
   <conditionalFormatting sqref="H10:I11">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">

</xml_diff>